<commit_message>
Add additional formats for Awareness Program Certificate files
</commit_message>
<xml_diff>
--- a/docs/Awareness Program Certificate - Data.xlsx
+++ b/docs/Awareness Program Certificate - Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Graphics\Certificates\awareness program\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hussain\Documents\GitHub\map.certificate\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8429C02-C0ED-4C52-8715-1E921E0392C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B22A6CA-6B19-4244-986C-27C8C82EDCED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11B0BF22-8D73-41F2-B77D-A5D147A672BC}"/>
+    <workbookView xWindow="22932" yWindow="-17700" windowWidth="17496" windowHeight="30216" xr2:uid="{11B0BF22-8D73-41F2-B77D-A5D147A672BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -177,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -189,11 +189,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Faruma"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -212,20 +232,6 @@
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Faruma"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -243,10 +249,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D43AA190-5A1C-43D7-8576-92E31EED0159}" name="Table1" displayName="Table1" ref="A1:F64" totalsRowShown="0">
   <autoFilter ref="A1:F64" xr:uid="{D43AA190-5A1C-43D7-8576-92E31EED0159}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C5417838-AE48-4290-8594-E67988BEF349}" name="#"/>
-    <tableColumn id="2" xr3:uid="{53E3FC65-DA71-4ED1-B3BE-24B5B04898C7}" name="Name" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{25CF85B1-1883-4C6A-BEC3-101DFDD30C03}" name="ID" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{AA1F0425-9808-468C-A189-738652856CC5}" name="Year" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C5417838-AE48-4290-8594-E67988BEF349}" name="#" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{53E3FC65-DA71-4ED1-B3BE-24B5B04898C7}" name="Name" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{25CF85B1-1883-4C6A-BEC3-101DFDD30C03}" name="ID" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{AA1F0425-9808-468C-A189-738652856CC5}" name="Year" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{8FA670C8-9C41-402E-AB22-96883D961C2C}" name="Month"/>
     <tableColumn id="6" xr3:uid="{C4410BFD-FEB7-496B-9107-FECD9913A6A2}" name="Day"/>
   </tableColumns>
@@ -574,7 +580,7 @@
   <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.65"/>
@@ -611,10 +617,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -623,18 +629,18 @@
       <c r="D2" s="3">
         <v>2025</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -643,18 +649,18 @@
       <c r="D3" s="3">
         <v>2025</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -663,18 +669,18 @@
       <c r="D4" s="3">
         <v>2025</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -683,18 +689,18 @@
       <c r="D5" s="3">
         <v>2025</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -703,18 +709,18 @@
       <c r="D6" s="3">
         <v>2025</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -723,18 +729,18 @@
       <c r="D7" s="3">
         <v>2025</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -743,18 +749,18 @@
       <c r="D8" s="3">
         <v>2025</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -763,18 +769,18 @@
       <c r="D9" s="3">
         <v>2025</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -783,18 +789,18 @@
       <c r="D10" s="3">
         <v>2025</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -803,18 +809,18 @@
       <c r="D11" s="3">
         <v>2025</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -823,277 +829,277 @@
       <c r="D12" s="3">
         <v>2025</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A14">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A15">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A16">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.65">
-      <c r="A17">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.65">
-      <c r="A18">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.65">
-      <c r="A19">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.65">
-      <c r="A20">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.65">
-      <c r="A21">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.65">
-      <c r="A22">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.65">
-      <c r="A23">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.65">
-      <c r="A24">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.65">
-      <c r="A25">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.65">
-      <c r="A26">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.65">
-      <c r="A27">
+      <c r="A27" s="3">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.65">
-      <c r="A28">
+      <c r="A28" s="3">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.65">
-      <c r="A29">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.65">
-      <c r="A30">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.65">
-      <c r="A31">
+      <c r="A31" s="3">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.65">
-      <c r="A32">
+      <c r="A32" s="3">
         <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A33">
+      <c r="A33" s="3">
         <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A34">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A35">
+      <c r="A35" s="3">
         <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A36">
+      <c r="A36" s="3">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A37">
+      <c r="A37" s="3">
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A38">
+      <c r="A38" s="3">
         <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A39">
+      <c r="A39" s="3">
         <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A40">
+      <c r="A40" s="3">
         <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A41">
+      <c r="A41" s="3">
         <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A42">
+      <c r="A42" s="3">
         <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A43">
+      <c r="A43" s="3">
         <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A44">
+      <c r="A44" s="3">
         <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A45">
+      <c r="A45" s="3">
         <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A46">
+      <c r="A46" s="3">
         <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A47">
+      <c r="A47" s="3">
         <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A48">
+      <c r="A48" s="3">
         <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A49">
+      <c r="A49" s="3">
         <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A50">
+      <c r="A50" s="3">
         <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A51">
+      <c r="A51" s="3">
         <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A52">
+      <c r="A52" s="3">
         <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A53">
+      <c r="A53" s="3">
         <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A54">
+      <c r="A54" s="3">
         <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A55">
+      <c r="A55" s="3">
         <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A56">
+      <c r="A56" s="3">
         <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A57">
+      <c r="A57" s="3">
         <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A58">
+      <c r="A58" s="3">
         <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A59">
+      <c r="A59" s="3">
         <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A60">
+      <c r="A60" s="3">
         <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A61">
+      <c r="A61" s="3">
         <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A62">
+      <c r="A62" s="3">
         <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A63">
+      <c r="A63" s="3">
         <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A64">
+      <c r="A64" s="3">
         <v>63</v>
       </c>
     </row>

</xml_diff>